<commit_message>
Completed sprint 1 execution chart and burndown
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint1/burndown.xlsx
+++ b/sprint_backlog/sprint1/burndown.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ADE918-D9AA-4730-8708-B9A4F8B9F378}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3482A-04C7-40E3-8F73-93E6A92C1B42}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Days</t>
   </si>
@@ -231,6 +231,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -240,13 +247,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,6 +262,1177 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Provisial (in story points)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0251-4074-94BC-7182BADC0821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual (in story points)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0251-4074-94BC-7182BADC0821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1221650767"/>
+        <c:axId val="1110143711"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1221650767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1110143711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1110143711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Story Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1221650767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5003CB6F-7393-44A1-A98A-EECBF5781674}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,27 +1701,27 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.05078125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -568,12 +1739,12 @@
       <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -591,27 +1762,38 @@
       <c r="F3" s="2">
         <v>18</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>20</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
+      <c r="C4" s="8">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8">
+        <v>16</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added sprint reports for sprints 1 and 2
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint1/burndown.xlsx
+++ b/sprint_backlog/sprint1/burndown.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3482A-04C7-40E3-8F73-93E6A92C1B42}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C7AC2-FDFB-4E19-8E37-02CFE27974D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Days</t>
   </si>
@@ -522,10 +522,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1399,15 +1399,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>280987</xdr:colOff>
+      <xdr:colOff>14287</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1701,7 +1701,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,10 +1783,10 @@
         <v>18</v>
       </c>
       <c r="F4" s="8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>